<commit_message>
adicionando os dados do inversor
</commit_message>
<xml_diff>
--- a/banco de modulos e inversores.xlsx
+++ b/banco de modulos e inversores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breno\Desktop\teste enviar arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breno\Desktop\teste enviar arquivos\memorial_automatizado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01524C4C-51D2-4ACF-A584-7AE022EB59FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EE769D-49A1-4369-A342-E75A2BACF135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modulos" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Fabricante</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>LEPTON</t>
+  </si>
+  <si>
+    <t>SOFAR</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L232"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -3964,12 +3967,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4FF4E62-5E7E-41B3-9CC0-AD15366E4981}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>